<commit_message>
Updated Tables structures - latest
</commit_message>
<xml_diff>
--- a/ERP_TableStructure.xlsx
+++ b/ERP_TableStructure.xlsx
@@ -15,7 +15,7 @@
     <sheet name="User Tables" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'User Tables'!$A$1:$H$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'User Tables'!$A$1:$H$55</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="73">
   <si>
     <t xml:space="preserve">TblUsers </t>
   </si>
@@ -50,15 +50,6 @@
     <t xml:space="preserve">user_id </t>
   </si>
   <si>
-    <t xml:space="preserve">username </t>
-  </si>
-  <si>
-    <t xml:space="preserve">email </t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>full_name</t>
   </si>
   <si>
@@ -68,12 +59,6 @@
     <t>phone_no</t>
   </si>
   <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>token</t>
-  </si>
-  <si>
     <t>is_active</t>
   </si>
   <si>
@@ -83,12 +68,6 @@
     <t>created_by</t>
   </si>
   <si>
-    <t>update_dt</t>
-  </si>
-  <si>
-    <t>update_by</t>
-  </si>
-  <si>
     <t>time_zone</t>
   </si>
   <si>
@@ -110,9 +89,6 @@
     <t>created_tm</t>
   </si>
   <si>
-    <t>update_tm</t>
-  </si>
-  <si>
     <t>time without time zone</t>
   </si>
   <si>
@@ -125,9 +101,6 @@
     <t>character varying(1)</t>
   </si>
   <si>
-    <t>character varying(30)</t>
-  </si>
-  <si>
     <t>character varying(15)</t>
   </si>
   <si>
@@ -188,18 +161,6 @@
     <t>can_update</t>
   </si>
   <si>
-    <t>parent</t>
-  </si>
-  <si>
-    <t>key1</t>
-  </si>
-  <si>
-    <t>key2</t>
-  </si>
-  <si>
-    <t>use</t>
-  </si>
-  <si>
     <t>chart_name</t>
   </si>
   <si>
@@ -243,6 +204,48 @@
   </si>
   <si>
     <t>UNIQUE(role_id, module_id, page_id, report_id, chart_id)</t>
+  </si>
+  <si>
+    <t>page_url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_name </t>
+  </si>
+  <si>
+    <t>user_password</t>
+  </si>
+  <si>
+    <t>user_token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_email </t>
+  </si>
+  <si>
+    <t>user_address</t>
+  </si>
+  <si>
+    <t>page_key1</t>
+  </si>
+  <si>
+    <t>page_key2</t>
+  </si>
+  <si>
+    <t>page_use</t>
+  </si>
+  <si>
+    <t>parent_page</t>
+  </si>
+  <si>
+    <t>updated_dt</t>
+  </si>
+  <si>
+    <t>updated_tm</t>
+  </si>
+  <si>
+    <t>updated_by</t>
+  </si>
+  <si>
+    <t>character varying(300)</t>
   </si>
 </sst>
 </file>
@@ -603,11 +606,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H53" sqref="H53"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -640,13 +643,13 @@
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -657,549 +660,605 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B35" s="3" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B36" s="3" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C38" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H38" s="4" t="s">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B37" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B39" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B40" s="3" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D42" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B41" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H42" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B43" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>23</v>
+      <c r="C43" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B44" s="3" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C45" s="1"/>
-    </row>
-    <row r="47" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C47" s="3" t="s">
+      <c r="B45" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C46" s="1"/>
+    </row>
+    <row r="48" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B50" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B51" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B52" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B53" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="B48" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C48" s="3" t="s">
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B54" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E48" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H48" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B49" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C49" s="3" t="s">
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B55" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E49" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B50" s="3" t="s">
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B56" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C56" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E50" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B51" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B52" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B53" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B54" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B55" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" s="1"/>
       <c r="B62" s="1" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A65" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H65" s="7" t="s">
-        <v>70</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B63" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="B66" s="1" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H66" s="7" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B67" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B68" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B69" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B70" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B71" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B72" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C67" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>34</v>
+      <c r="C72" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B73" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B74" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H54"/>
+  <autoFilter ref="A1:H55"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Migration Run Comment
</commit_message>
<xml_diff>
--- a/ERP_TableStructure.xlsx
+++ b/ERP_TableStructure.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7476" windowHeight="2808" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7476" windowHeight="2808" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="User Tables" sheetId="1" r:id="rId1"/>
     <sheet name="WEB_API" sheetId="2" r:id="rId2"/>
     <sheet name="Installed Packages" sheetId="3" r:id="rId3"/>
+    <sheet name="MIgrations" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'User Tables'!$A$1:$H$85</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="117">
   <si>
     <t xml:space="preserve">TblUsers </t>
   </si>
@@ -370,6 +371,18 @@
   <si>
     <t>System.IdentityModel.Tokens.Jwt</t>
   </si>
+  <si>
+    <t>Add-migration initialCreate1 -o "Migrations/Auth" -c "ERPDbContext"</t>
+  </si>
+  <si>
+    <t>dotnet ef database update --project "D:/Projects/DotNetCore/ERP_Backend/ERPDataAccess/ERPDataAccess.csproj" --startup-project "D:/Projects/DotNetCore/ERP_Backend/ERPWebAPI/ERPWebAPI.csproj" --context "ERPDbContext" --verbose</t>
+  </si>
+  <si>
+    <t>To Create Migration</t>
+  </si>
+  <si>
+    <t>To Update Migration</t>
+  </si>
 </sst>
 </file>
 
@@ -447,13 +460,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -11958,8 +11974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12104,4 +12120,39 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33.77734375" customWidth="1"/>
+    <col min="2" max="2" width="86.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>